<commit_message>
docu: pulseview tool for visualisation?
</commit_message>
<xml_diff>
--- a/docu.xlsx
+++ b/docu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwesTechnik\arduino-promini-analog-to-sdcard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E185CD3-FF24-4B18-9486-CAD80B197B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DE001D-5892-445A-BB31-C5D3494FBEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="0" windowWidth="20295" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="0" windowWidth="20295" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Which tool to view the data on the desktop PC?</t>
   </si>
@@ -127,6 +127,16 @@
   </si>
   <si>
     <t>bpm</t>
+  </si>
+  <si>
+    <t>https://sigrok.org/doc/pulseview/unstable/manual.html</t>
+  </si>
+  <si>
+    <t>PulseView (sigrok)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> free, open-source, and cross-platform.
+Reads many formats, also csv.</t>
   </si>
 </sst>
 </file>
@@ -179,10 +189,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -239,6 +252,50 @@
         <a:xfrm>
           <a:off x="8410408" y="2514600"/>
           <a:ext cx="2296448" cy="1848459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1175861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>572298</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1600659</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B19604C3-3D46-362E-3081-F3FE80D1EE7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8115300" y="5900261"/>
+          <a:ext cx="2991648" cy="1720198"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -513,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B2:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,6 +692,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="15" spans="2:6" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{1C82EB46-A223-46B6-B369-48939C4E2B1E}"/>
@@ -642,9 +710,10 @@
     <hyperlink ref="F8" r:id="rId3" xr:uid="{E1B2F9E0-A01D-40EB-8FE7-EA37AF711873}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{30828D57-1E6D-44AE-AAE3-44022168A29E}"/>
     <hyperlink ref="F13" r:id="rId5" xr:uid="{E193ADBA-E381-466A-9013-02172678E015}"/>
+    <hyperlink ref="F15" r:id="rId6" xr:uid="{3A96C839-BD99-4221-857B-75AB729F6871}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -652,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6907062F-DB08-49B3-BF65-049ECE8A022C}">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>